<commit_message>
Read Test data from Excel
</commit_message>
<xml_diff>
--- a/ui-tests/src/test/resources/test-data/TestData.xlsx
+++ b/ui-tests/src/test/resources/test-data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Automation\Automation-testng\ui-tests\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DD8223C-3948-4FC6-9C4C-FB088EFE718D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E537CBAC-D943-40D5-8AC8-03DF11BED318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F21F4E43-5122-4267-8231-7C967DA2273F}"/>
   </bookViews>
@@ -34,12 +34,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,13 +81,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,12 +403,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4007B2-3D47-42D9-A19D-A9E0189D63F0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{8D3099A4-BB45-49D8-9C8E-B215476F7AA6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Execl and Email changes
</commit_message>
<xml_diff>
--- a/ui-tests/src/test/resources/test-data/TestData.xlsx
+++ b/ui-tests/src/test/resources/test-data/TestData.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Automation\Automation-testng\ui-tests\src\test\resources\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E537CBAC-D943-40D5-8AC8-03DF11BED318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F21F4E43-5122-4267-8231-7C967DA2273F}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,30 +29,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>URL</t>
+    <t>Username</t>
   </si>
   <si>
-    <t>https://www.google.com</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,16 +70,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -149,7 +135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -201,7 +187,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -395,34 +381,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4007B2-3D47-42D9-A19D-A9E0189D63F0}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{8D3099A4-BB45-49D8-9C8E-B215476F7AA6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>